<commit_message>
Copied 7.2.1 files over.
</commit_message>
<xml_diff>
--- a/beams-test-results.xlsx
+++ b/beams-test-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/Katalon Studio/Exede_Beam_Tests_v2.1 copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B84138D3-B563-1240-B449-8319BB017707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A27FDB0-95D1-A443-A308-7944F8A06200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73940" yWindow="-15660" windowWidth="33600" windowHeight="20540" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Moving to JH github - Ran test locally to update Test scripts / paths.
</commit_message>
<xml_diff>
--- a/beams-test-results.xlsx
+++ b/beams-test-results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/Katalon Studio/Exede_Beam_Tests_v2.1 copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A27FDB0-95D1-A443-A308-7944F8A06200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7A27FDB0-95D1-A443-A308-7944F8A06200}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}"/>
+    <workbookView windowHeight="19440" windowWidth="33600" xWindow="0" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,11 +31,136 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="41">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>BEAM</t>
+  </si>
+  <si>
+    <t>UFF</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>API PLAN</t>
+  </si>
+  <si>
+    <t>beam 65 zip 58438 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>liberty12</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>beam 65 zip 56740 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 67 zip 49916 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 79 zip 04763 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 95 zip 33040 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>beam 301 zip 55806 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>gold30</t>
+  </si>
+  <si>
+    <t>beam 302 zip 56440 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 303 zip 54701 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 304 zip 54124 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 305 zip 48661 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 309 zip 50126 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 310 zip 61032 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 311 zip 47963 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 312 zip 46777 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 314 zip 13730 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 315 zip 12208 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>liberty12-unlimited</t>
+  </si>
+  <si>
+    <t>beam 317 zip 62702 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 319 zip 45414 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 322 zip 08724 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 325 zip 72401 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 327 zip 40744 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 328 zip 24121 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 330 zip 73505 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 332 zip 71603 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 333 zip 38901 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 334 zip 35758 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 336 zip 29204 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -71,15 +196,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -103,7 +228,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -120,10 +245,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -158,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -210,7 +335,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -321,21 +446,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -352,7 +477,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -404,222 +529,498 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566AE47B-A227-3843-B403-5EAFB2F47EB5}">
-  <dimension ref="A1:E542"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566AE47B-A227-3843-B403-5EAFB2F47EB5}">
+  <dimension ref="A1:F542"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.83203125" style="1" collapsed="1"/>
-    <col min="4" max="4" width="24.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="58.33203125" collapsed="true"/>
+    <col min="2" max="3" style="1" width="10.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="24.1640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1"/>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28"/>
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29"/>
@@ -2252,14 +2653,14 @@
       <c r="D261"/>
       <c r="E261"/>
     </row>
-    <row r="262" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row outlineLevel="1" r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262"/>
       <c r="B262"/>
       <c r="C262"/>
       <c r="D262"/>
       <c r="E262"/>
     </row>
-    <row r="263" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row outlineLevel="1" r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263"/>
       <c r="B263"/>
       <c r="C263"/>
@@ -4223,15 +4624,15 @@
     <sortCondition ref="A2:A264"/>
   </sortState>
   <conditionalFormatting sqref="B134:C1048576 B1:C132">
-    <cfRule type="beginsWith" dxfId="1" priority="3" operator="beginsWith" text="F">
+    <cfRule dxfId="1" operator="beginsWith" priority="3" text="F" type="beginsWith">
       <formula>LEFT(B1,LEN("F"))="F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B133:C133">
-    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="F">
+    <cfRule dxfId="0" operator="beginsWith" priority="1" text="F" type="beginsWith">
       <formula>LEFT(B133,LEN("F"))="F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clearing out Test data.
</commit_message>
<xml_diff>
--- a/beams-test-results.xlsx
+++ b/beams-test-results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/Katalon Studio/Exede_Beam_Tests_v2.1 copy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/jenkins-beam-tests-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{7A27FDB0-95D1-A443-A308-7944F8A06200}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED523548-272E-E644-A528-20138E1F1EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="19440" windowWidth="33600" xWindow="0" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,136 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="41">
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>BEAM</t>
-  </si>
-  <si>
-    <t>UFF</t>
-  </si>
-  <si>
-    <t>PLAN</t>
-  </si>
-  <si>
-    <t>API PLAN</t>
-  </si>
-  <si>
-    <t>beam 65 zip 58438 upfront fees 0 plan Augmented Standard Plan</t>
-  </si>
-  <si>
-    <t>Augmented Standard Plan</t>
-  </si>
-  <si>
-    <t>liberty12</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>beam 65 zip 56740 upfront fees 0 plan Augmented Standard Plan</t>
-  </si>
-  <si>
-    <t>beam 67 zip 49916 upfront fees 0 plan Augmented Standard Plan</t>
-  </si>
-  <si>
-    <t>beam 79 zip 04763 upfront fees 0 plan Augmented Standard Plan</t>
-  </si>
-  <si>
-    <t>beam 95 zip 33040 upfront fees 0 plan Augmented Standard Plan</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>beam 301 zip 55806 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>gold30</t>
-  </si>
-  <si>
-    <t>beam 302 zip 56440 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 303 zip 54701 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 304 zip 54124 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 305 zip 48661 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 309 zip 50126 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 310 zip 61032 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 311 zip 47963 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 312 zip 46777 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 314 zip 13730 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 315 zip 12208 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>liberty12-unlimited</t>
-  </si>
-  <si>
-    <t>beam 317 zip 62702 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 319 zip 45414 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 322 zip 08724 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 325 zip 72401 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 327 zip 40744 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 328 zip 24121 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 330 zip 73505 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 332 zip 71603 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 333 zip 38901 upfront fees 0 plan VS2 Standard Offer</t>
-  </si>
-  <si>
-    <t>beam 334 zip 35758 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-  <si>
-    <t>beam 336 zip 29204 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -196,15 +71,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -228,7 +103,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -245,10 +120,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -283,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -335,7 +210,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -446,21 +321,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -477,7 +352,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -529,498 +404,222 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566AE47B-A227-3843-B403-5EAFB2F47EB5}">
-  <dimension ref="A1:F542"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566AE47B-A227-3843-B403-5EAFB2F47EB5}">
+  <dimension ref="A1:E542"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="58.33203125" collapsed="true"/>
-    <col min="2" max="3" style="1" width="10.83203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="24.1640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="58.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.83203125" style="1" collapsed="1"/>
+    <col min="4" max="4" width="24.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>29</v>
-      </c>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
-      </c>
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
+      <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" t="s">
-        <v>17</v>
-      </c>
+      <c r="D28"/>
+      <c r="E28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29"/>
@@ -2653,14 +2252,14 @@
       <c r="D261"/>
       <c r="E261"/>
     </row>
-    <row outlineLevel="1" r="262" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A262"/>
       <c r="B262"/>
       <c r="C262"/>
       <c r="D262"/>
       <c r="E262"/>
     </row>
-    <row outlineLevel="1" r="263" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A263"/>
       <c r="B263"/>
       <c r="C263"/>
@@ -4624,15 +4223,15 @@
     <sortCondition ref="A2:A264"/>
   </sortState>
   <conditionalFormatting sqref="B134:C1048576 B1:C132">
-    <cfRule dxfId="1" operator="beginsWith" priority="3" text="F" type="beginsWith">
+    <cfRule type="beginsWith" dxfId="1" priority="3" operator="beginsWith" text="F">
       <formula>LEFT(B1,LEN("F"))="F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B133:C133">
-    <cfRule dxfId="0" operator="beginsWith" priority="1" text="F" type="beginsWith">
+    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="F">
       <formula>LEFT(B133,LEN("F"))="F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made test case path Relative.
</commit_message>
<xml_diff>
--- a/beams-test-results.xlsx
+++ b/beams-test-results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhampleman/jenkins-beam-tests-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED523548-272E-E644-A528-20138E1F1EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{ED523548-272E-E644-A528-20138E1F1EEC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}"/>
+    <workbookView windowHeight="19440" windowWidth="33600" xWindow="0" xr2:uid="{8DECE85A-BF63-6B4C-B6D4-2E95F0A50A69}" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,11 +31,514 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="167">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>BEAM</t>
+  </si>
+  <si>
+    <t>UFF</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>API PLAN</t>
+  </si>
+  <si>
+    <t>beam 65 zip 58438 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>liberty12</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>beam 65 zip 56740 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 67 zip 49916 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 79 zip 04763 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 95 zip 33040 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 301 zip 55806 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>gold30</t>
+  </si>
+  <si>
+    <t>beam 302 zip 56440 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 303 zip 54701 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 304 zip 54124 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 305 zip 48661 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 309 zip 50126 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 310 zip 61032 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 311 zip 47963 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 312 zip 46777 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 314 zip 13730 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 315 zip 12208 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>liberty12-unlimited</t>
+  </si>
+  <si>
+    <t>beam 317 zip 62702 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 319 zip 45414 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 322 zip 08724 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 325 zip 72401 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 327 zip 40744 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 328 zip 24121 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 330 zip 73505 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 332 zip 71603 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 333 zip 38901 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 334 zip 35758 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 336 zip 29204 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 337 zip 27858 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 339 zip 75961 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 341 zip 39305 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 342 zip 36037 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 343 zip 31201 upfront fees 100 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 344 zip 29554 upfront fees 0 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 345 zip 78643 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 347 zip 70601 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 348 zip 70065 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 349 zip 39507 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 350 zip 32428 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 351 zip 32207 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 357 zip 99501 upfront fees 150 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 359 zip 32940 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 361 zip 96720 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 362 zip 78375 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 363 zip 85041 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 364 zip 95407 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 366 zip 98377 upfront fees 150 plan $50 OPP Liberty 12/25/50</t>
+  </si>
+  <si>
+    <t>$50 OPP Liberty 12/25/50</t>
+  </si>
+  <si>
+    <t>liberty12-wifi</t>
+  </si>
+  <si>
+    <t>beam 367 zip 97402 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 368 zip 95548 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 369 zip 93905 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 370 zip 93301 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 371 zip 91204 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 372 zip 92262 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>beam 447 zip 04774 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>gold12</t>
+  </si>
+  <si>
+    <t>beam 448 zip 04736 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 457 zip 97850 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 458 zip 59829 upfront fees 150 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 459 zip 59101 upfront fees 150 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 153 zip 59101 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 460 zip 57724 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 461 zip 56256 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 467 zip 04765 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 478 zip 96101 upfront fees 150 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 479 zip 83301 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 480 zip 82070 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 481 zip 67731 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 482 zip 68434 upfront fees 100 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 486 zip 16601 upfront fees 150 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 495 zip 93514 upfront fees 100 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 496 zip 84770 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 497 zip 81507 upfront fees 100 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 73 zip 81507 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 498 zip 67952 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 499 zip 67152 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 500 zip 65775 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 324 zip 65775 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 501 zip 38242 upfront fees 150 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 326 zip 38242 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 504 zip 27855 upfront fees 150 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 329 zip 27855 upfront fees 150 plan Liberty 12/25/50/Unlimited</t>
+  </si>
+  <si>
+    <t>beam 508 zip 93527 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 509 zip 86403 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 81 zip 86403 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 510 zip 87801 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 511 zip 79404 upfront fees 150 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 524 zip 79735 upfront fees 100 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 525 zip 76849 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 543 zip 33071 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 360 zip 33071 upfront fees 0 plan Augmented Standard Plan</t>
+  </si>
+  <si>
+    <t>beam 701 zip 95110 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>plat100</t>
+  </si>
+  <si>
+    <t>beam 702 zip 91935 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 703 zip 89523 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 704 zip 89019 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>gold50</t>
+  </si>
+  <si>
+    <t>beam 705 zip 85145 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 706 zip 97045 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 707 zip 79838 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 708 zip 84017 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 709 zip 87113 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 710 zip 59632 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 711 zip 80112 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 712 zip 78570 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 713 zip 78130 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 714 zip 57738 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 715 zip 75229 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 716 zip 73049 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 717 zip 77429 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 718 zip 68025 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 719 zip 64080 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 720 zip 72015 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 721 zip 50313 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 722 zip 38017 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 723 zip 55401 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 724 zip 62295 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 725 zip 35020 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 727 zip 53214 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 728 zip 46183 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 729 zip 30084 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 730 zip 43113 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 731 zip 29831 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 732 zip 48503 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 733 zip 28602 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 734 zip 15301 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 735 zip 27597 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 736 zip 23310 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 737 zip 18634 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 738 zip 02113 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 745 zip 92394 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 746 zip 95932 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 364 zip 95932 upfront fees 150 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 747 zip 97470 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 749 zip 98901 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 752 zip 80477 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 757 zip 76366 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 771 zip 63703 upfront fees 0 plan VS2 High Fill</t>
+  </si>
+  <si>
+    <t>beam 773 zip 61944 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 774 zip 36832 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 775 zip 54401 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 777 zip 31768 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 778 zip 49892 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 779 zip 40601 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 780 zip 46601 upfront fees 0 plan VS2 Best Offer A</t>
+  </si>
+  <si>
+    <t>beam 781 zip 37938 upfront fees 0 plan VS2 Best Offer B</t>
+  </si>
+  <si>
+    <t>beam 782 zip 34711 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 782 zip 32102 upfront fees 0 plan VS2 Standard Offer</t>
+  </si>
+  <si>
+    <t>beam 711 zip 80403 upfront fees 0 plan END</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -71,15 +574,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -103,7 +606,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -120,10 +623,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -158,7 +661,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -210,7 +713,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -321,21 +824,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -352,7 +855,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -404,1041 +907,2487 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566AE47B-A227-3843-B403-5EAFB2F47EB5}">
-  <dimension ref="A1:E542"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566AE47B-A227-3843-B403-5EAFB2F47EB5}">
+  <dimension ref="A1:F542"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.83203125" style="1" collapsed="1"/>
-    <col min="4" max="4" width="24.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="58.33203125" collapsed="true"/>
+    <col min="2" max="3" style="1" width="10.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="24.1640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="17.0" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1"/>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45"/>
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
+      <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="D51"/>
-      <c r="E51"/>
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="D52"/>
-      <c r="E52"/>
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
+      <c r="A55" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="D57"/>
-      <c r="E57"/>
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
-      <c r="E58"/>
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
-      <c r="E59"/>
+      <c r="A59" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
+      <c r="A62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
+      <c r="A64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
+      <c r="A65" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>64</v>
+      </c>
+      <c r="E65" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
+      <c r="A66" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" t="s">
+        <v>64</v>
+      </c>
+      <c r="E67" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
+      <c r="A68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
+      <c r="A69" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
+      <c r="A70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
+      <c r="A71" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" t="s">
+        <v>68</v>
+      </c>
+      <c r="D71" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72"/>
+      <c r="A72" t="s">
+        <v>88</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73"/>
-      <c r="E73"/>
+      <c r="A73" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>64</v>
+      </c>
+      <c r="E73" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="D74"/>
-      <c r="E74"/>
+      <c r="A74" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="D75"/>
-      <c r="E75"/>
+      <c r="A75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" t="s">
+        <v>68</v>
+      </c>
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
-      <c r="D76"/>
-      <c r="E76"/>
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
-      <c r="D77"/>
-      <c r="E77"/>
+      <c r="A77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B77" t="s">
+        <v>68</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="D78"/>
-      <c r="E78"/>
+      <c r="A78" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="D79"/>
-      <c r="E79"/>
+      <c r="A79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" t="s">
+        <v>64</v>
+      </c>
+      <c r="E79" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
+      <c r="A80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
+      <c r="A81" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>64</v>
+      </c>
+      <c r="E81" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
+      <c r="A82" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" t="s">
+        <v>68</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="D83"/>
-      <c r="E83"/>
+      <c r="A83" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84"/>
-      <c r="E84"/>
+      <c r="A84" t="s">
+        <v>100</v>
+      </c>
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>64</v>
+      </c>
+      <c r="E84" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
+      <c r="A85" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>64</v>
+      </c>
+      <c r="E85" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
-      <c r="D86"/>
-      <c r="E86"/>
+      <c r="A86" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>64</v>
+      </c>
+      <c r="E86" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
-      <c r="D87"/>
-      <c r="E87"/>
+      <c r="A87" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>64</v>
+      </c>
+      <c r="E87" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88"/>
+      <c r="A88" t="s">
+        <v>104</v>
+      </c>
+      <c r="B88" t="s">
+        <v>68</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" t="s">
+        <v>64</v>
+      </c>
+      <c r="E88" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89"/>
+      <c r="A89" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="D90"/>
-      <c r="E90"/>
+      <c r="A90" t="s">
+        <v>106</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" t="s">
+        <v>107</v>
+      </c>
+      <c r="E90" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
-      <c r="D91"/>
-      <c r="E91"/>
+      <c r="A91" t="s">
+        <v>109</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>107</v>
+      </c>
+      <c r="E91" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-      <c r="D92"/>
-      <c r="E92"/>
+      <c r="A92" t="s">
+        <v>110</v>
+      </c>
+      <c r="B92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>107</v>
+      </c>
+      <c r="E92" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93"/>
+      <c r="A93" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>112</v>
+      </c>
+      <c r="E93" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="D94"/>
-      <c r="E94"/>
+      <c r="A94" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>112</v>
+      </c>
+      <c r="E94" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-      <c r="D95"/>
-      <c r="E95"/>
+      <c r="A95" t="s">
+        <v>115</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>107</v>
+      </c>
+      <c r="E95" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
-      <c r="D96"/>
-      <c r="E96"/>
+      <c r="A96" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" t="s">
+        <v>107</v>
+      </c>
+      <c r="E96" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97"/>
-      <c r="B97"/>
-      <c r="C97"/>
-      <c r="D97"/>
-      <c r="E97"/>
+      <c r="A97" t="s">
+        <v>117</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>107</v>
+      </c>
+      <c r="E97" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="C98"/>
-      <c r="D98"/>
-      <c r="E98"/>
+      <c r="A98" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>107</v>
+      </c>
+      <c r="E98" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="C99"/>
-      <c r="D99"/>
-      <c r="E99"/>
+      <c r="A99" t="s">
+        <v>119</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" t="s">
+        <v>107</v>
+      </c>
+      <c r="E99" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
-      <c r="D100"/>
-      <c r="E100"/>
+      <c r="A100" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" t="s">
+        <v>107</v>
+      </c>
+      <c r="E100" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
-      <c r="D101"/>
-      <c r="E101"/>
+      <c r="A101" t="s">
+        <v>121</v>
+      </c>
+      <c r="B101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" t="s">
+        <v>107</v>
+      </c>
+      <c r="E101" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102"/>
+      <c r="A102" t="s">
+        <v>122</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" t="s">
+        <v>107</v>
+      </c>
+      <c r="E102" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-      <c r="D103"/>
-      <c r="E103"/>
+      <c r="A103" t="s">
+        <v>123</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103" t="s">
+        <v>112</v>
+      </c>
+      <c r="E103" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-      <c r="D104"/>
-      <c r="E104"/>
+      <c r="A104" t="s">
+        <v>124</v>
+      </c>
+      <c r="B104" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
-      <c r="D105"/>
-      <c r="E105"/>
+      <c r="A105" t="s">
+        <v>125</v>
+      </c>
+      <c r="B105" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>107</v>
+      </c>
+      <c r="E105" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106"/>
-      <c r="D106"/>
-      <c r="E106"/>
+      <c r="A106" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="C107"/>
-      <c r="D107"/>
-      <c r="E107"/>
+      <c r="A107" t="s">
+        <v>127</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" t="s">
+        <v>107</v>
+      </c>
+      <c r="E107" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="C108"/>
-      <c r="D108"/>
-      <c r="E108"/>
+      <c r="A108" t="s">
+        <v>128</v>
+      </c>
+      <c r="B108" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" t="s">
+        <v>107</v>
+      </c>
+      <c r="E108" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109"/>
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109"/>
+      <c r="A109" t="s">
+        <v>129</v>
+      </c>
+      <c r="B109" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" t="s">
+        <v>107</v>
+      </c>
+      <c r="E109" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110"/>
-      <c r="B110"/>
-      <c r="C110"/>
-      <c r="D110"/>
-      <c r="E110"/>
+      <c r="A110" t="s">
+        <v>130</v>
+      </c>
+      <c r="B110" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" t="s">
+        <v>107</v>
+      </c>
+      <c r="E110" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111"/>
-      <c r="B111"/>
-      <c r="C111"/>
-      <c r="D111"/>
-      <c r="E111"/>
+      <c r="A111" t="s">
+        <v>131</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" t="s">
+        <v>112</v>
+      </c>
+      <c r="E111" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112"/>
-      <c r="B112"/>
-      <c r="C112"/>
-      <c r="D112"/>
-      <c r="E112"/>
+      <c r="A112" t="s">
+        <v>132</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" t="s">
+        <v>107</v>
+      </c>
+      <c r="E112" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="C113"/>
-      <c r="D113"/>
-      <c r="E113"/>
+      <c r="A113" t="s">
+        <v>133</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" t="s">
+        <v>9</v>
+      </c>
+      <c r="D113" t="s">
+        <v>107</v>
+      </c>
+      <c r="E113" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="C114"/>
-      <c r="D114"/>
-      <c r="E114"/>
+      <c r="A114" t="s">
+        <v>134</v>
+      </c>
+      <c r="B114" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>107</v>
+      </c>
+      <c r="E114" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="C115"/>
-      <c r="D115"/>
-      <c r="E115"/>
+      <c r="A115" t="s">
+        <v>135</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" t="s">
+        <v>107</v>
+      </c>
+      <c r="E115" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="C116"/>
-      <c r="D116"/>
-      <c r="E116"/>
+      <c r="A116" t="s">
+        <v>136</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" t="s">
+        <v>107</v>
+      </c>
+      <c r="E116" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="C117"/>
-      <c r="D117"/>
-      <c r="E117"/>
+      <c r="A117" t="s">
+        <v>137</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" t="s">
+        <v>107</v>
+      </c>
+      <c r="E117" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="C118"/>
-      <c r="D118"/>
-      <c r="E118"/>
+      <c r="A118" t="s">
+        <v>138</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
-      <c r="D119"/>
-      <c r="E119"/>
+      <c r="A119" t="s">
+        <v>139</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
-      <c r="D120"/>
-      <c r="E120"/>
+      <c r="A120" t="s">
+        <v>140</v>
+      </c>
+      <c r="B120" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121"/>
-      <c r="B121"/>
-      <c r="C121"/>
-      <c r="D121"/>
-      <c r="E121"/>
+      <c r="A121" t="s">
+        <v>141</v>
+      </c>
+      <c r="B121" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" t="s">
+        <v>112</v>
+      </c>
+      <c r="E121" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122"/>
-      <c r="B122"/>
-      <c r="C122"/>
-      <c r="D122"/>
-      <c r="E122"/>
+      <c r="A122" t="s">
+        <v>142</v>
+      </c>
+      <c r="B122" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" t="s">
+        <v>112</v>
+      </c>
+      <c r="E122" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="C123"/>
-      <c r="D123"/>
-      <c r="E123"/>
+      <c r="A123" t="s">
+        <v>143</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" t="s">
+        <v>64</v>
+      </c>
+      <c r="E123" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="C124"/>
-      <c r="D124"/>
-      <c r="E124"/>
+      <c r="A124" t="s">
+        <v>144</v>
+      </c>
+      <c r="B124" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125"/>
-      <c r="B125"/>
-      <c r="C125"/>
-      <c r="D125"/>
-      <c r="E125"/>
+      <c r="A125" t="s">
+        <v>145</v>
+      </c>
+      <c r="B125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" t="s">
+        <v>112</v>
+      </c>
+      <c r="E125" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126"/>
-      <c r="B126"/>
-      <c r="C126"/>
-      <c r="D126"/>
-      <c r="E126"/>
+      <c r="A126" t="s">
+        <v>146</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D126" t="s">
+        <v>112</v>
+      </c>
+      <c r="E126" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127"/>
-      <c r="B127"/>
-      <c r="C127"/>
-      <c r="D127"/>
-      <c r="E127"/>
+      <c r="A127" t="s">
+        <v>147</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" t="s">
+        <v>9</v>
+      </c>
+      <c r="D127" t="s">
+        <v>15</v>
+      </c>
+      <c r="E127" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128"/>
-      <c r="B128"/>
-      <c r="C128"/>
-      <c r="D128"/>
-      <c r="E128"/>
+      <c r="A128" t="s">
+        <v>148</v>
+      </c>
+      <c r="B128" t="s">
+        <v>68</v>
+      </c>
+      <c r="C128" t="s">
+        <v>68</v>
+      </c>
+      <c r="D128" t="s">
+        <v>112</v>
+      </c>
+      <c r="E128" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129"/>
-      <c r="B129"/>
-      <c r="C129"/>
-      <c r="D129"/>
-      <c r="E129"/>
+      <c r="A129" t="s">
+        <v>149</v>
+      </c>
+      <c r="B129" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" t="s">
+        <v>9</v>
+      </c>
+      <c r="D129" t="s">
+        <v>112</v>
+      </c>
+      <c r="E129" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130"/>
-      <c r="B130"/>
-      <c r="C130"/>
-      <c r="D130"/>
-      <c r="E130"/>
+      <c r="A130" t="s">
+        <v>150</v>
+      </c>
+      <c r="B130" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130" t="s">
+        <v>112</v>
+      </c>
+      <c r="E130" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131"/>
-      <c r="B131"/>
-      <c r="C131"/>
-      <c r="D131"/>
-      <c r="E131"/>
+      <c r="A131" t="s">
+        <v>151</v>
+      </c>
+      <c r="B131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" t="s">
+        <v>9</v>
+      </c>
+      <c r="D131" t="s">
+        <v>112</v>
+      </c>
+      <c r="E131" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132"/>
-      <c r="B132"/>
-      <c r="C132"/>
-      <c r="D132"/>
-      <c r="E132"/>
+      <c r="A132" t="s">
+        <v>152</v>
+      </c>
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" t="s">
+        <v>112</v>
+      </c>
+      <c r="E132" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133"/>
-      <c r="B133"/>
-      <c r="C133"/>
-      <c r="D133"/>
-      <c r="E133"/>
+      <c r="A133" t="s">
+        <v>153</v>
+      </c>
+      <c r="B133" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" t="s">
+        <v>15</v>
+      </c>
+      <c r="E133" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134"/>
-      <c r="B134"/>
-      <c r="C134"/>
-      <c r="D134"/>
-      <c r="E134"/>
+      <c r="A134" t="s">
+        <v>154</v>
+      </c>
+      <c r="B134" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" t="s">
+        <v>9</v>
+      </c>
+      <c r="D134" t="s">
+        <v>64</v>
+      </c>
+      <c r="E134" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135"/>
-      <c r="B135"/>
-      <c r="C135"/>
-      <c r="D135"/>
-      <c r="E135"/>
+      <c r="A135" t="s">
+        <v>155</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" t="s">
+        <v>9</v>
+      </c>
+      <c r="D135" t="s">
+        <v>15</v>
+      </c>
+      <c r="E135" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136"/>
-      <c r="B136"/>
-      <c r="C136"/>
-      <c r="D136"/>
-      <c r="E136"/>
+      <c r="A136" t="s">
+        <v>156</v>
+      </c>
+      <c r="B136" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" t="s">
+        <v>15</v>
+      </c>
+      <c r="E136" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137"/>
-      <c r="B137"/>
-      <c r="C137"/>
-      <c r="D137"/>
-      <c r="E137"/>
+      <c r="A137" t="s">
+        <v>157</v>
+      </c>
+      <c r="B137" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" t="s">
+        <v>9</v>
+      </c>
+      <c r="D137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E137" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138"/>
-      <c r="B138"/>
-      <c r="C138"/>
-      <c r="D138"/>
-      <c r="E138"/>
+      <c r="A138" t="s">
+        <v>158</v>
+      </c>
+      <c r="B138" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138" t="s">
+        <v>9</v>
+      </c>
+      <c r="D138" t="s">
+        <v>107</v>
+      </c>
+      <c r="E138" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139"/>
-      <c r="B139"/>
-      <c r="C139"/>
-      <c r="D139"/>
-      <c r="E139"/>
+      <c r="A139" t="s">
+        <v>159</v>
+      </c>
+      <c r="B139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" t="s">
+        <v>9</v>
+      </c>
+      <c r="D139" t="s">
+        <v>107</v>
+      </c>
+      <c r="E139" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140"/>
-      <c r="B140"/>
-      <c r="C140"/>
-      <c r="D140"/>
-      <c r="E140"/>
+      <c r="A140" t="s">
+        <v>160</v>
+      </c>
+      <c r="B140" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" t="s">
+        <v>9</v>
+      </c>
+      <c r="D140" t="s">
+        <v>112</v>
+      </c>
+      <c r="E140" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141"/>
-      <c r="B141"/>
-      <c r="C141"/>
-      <c r="D141"/>
-      <c r="E141"/>
+      <c r="A141" t="s">
+        <v>161</v>
+      </c>
+      <c r="B141" t="s">
+        <v>9</v>
+      </c>
+      <c r="C141" t="s">
+        <v>9</v>
+      </c>
+      <c r="D141" t="s">
+        <v>112</v>
+      </c>
+      <c r="E141" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142"/>
-      <c r="B142"/>
-      <c r="C142"/>
-      <c r="D142"/>
-      <c r="E142"/>
+      <c r="A142" t="s">
+        <v>162</v>
+      </c>
+      <c r="B142" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" t="s">
+        <v>107</v>
+      </c>
+      <c r="E142" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143"/>
-      <c r="B143"/>
-      <c r="C143"/>
-      <c r="D143"/>
-      <c r="E143"/>
+      <c r="A143" t="s">
+        <v>163</v>
+      </c>
+      <c r="B143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" t="s">
+        <v>15</v>
+      </c>
+      <c r="E143" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144"/>
-      <c r="B144"/>
-      <c r="C144"/>
-      <c r="D144"/>
-      <c r="E144"/>
+      <c r="A144" t="s">
+        <v>164</v>
+      </c>
+      <c r="B144" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" t="s">
+        <v>9</v>
+      </c>
+      <c r="D144" t="s">
+        <v>15</v>
+      </c>
+      <c r="E144" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145"/>
+      <c r="A145" t="s">
+        <v>165</v>
+      </c>
       <c r="B145"/>
       <c r="C145"/>
-      <c r="D145"/>
-      <c r="E145"/>
+      <c r="D145" t="s">
+        <v>166</v>
+      </c>
+      <c r="E145" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146"/>
@@ -2252,14 +4201,14 @@
       <c r="D261"/>
       <c r="E261"/>
     </row>
-    <row r="262" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row outlineLevel="1" r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262"/>
       <c r="B262"/>
       <c r="C262"/>
       <c r="D262"/>
       <c r="E262"/>
     </row>
-    <row r="263" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row outlineLevel="1" r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263"/>
       <c r="B263"/>
       <c r="C263"/>
@@ -4223,15 +6172,15 @@
     <sortCondition ref="A2:A264"/>
   </sortState>
   <conditionalFormatting sqref="B134:C1048576 B1:C132">
-    <cfRule type="beginsWith" dxfId="1" priority="3" operator="beginsWith" text="F">
+    <cfRule dxfId="1" operator="beginsWith" priority="3" text="F" type="beginsWith">
       <formula>LEFT(B1,LEN("F"))="F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B133:C133">
-    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="F">
+    <cfRule dxfId="0" operator="beginsWith" priority="1" text="F" type="beginsWith">
       <formula>LEFT(B133,LEN("F"))="F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>